<commit_message>
Update Spatial configuration table.xlsx
</commit_message>
<xml_diff>
--- a/documentation/Spatial configuration table.xlsx
+++ b/documentation/Spatial configuration table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tud365-my.sharepoint.com/personal/serenst_tudelft_nl/Documents/spatial computing architecture/CDS-Project/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="231" documentId="8_{697A1238-A541-4A1D-8A1B-4D07BCAF2535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7251A077-0718-4526-9978-45032BBD417D}"/>
+  <xr:revisionPtr revIDLastSave="272" documentId="8_{697A1238-A541-4A1D-8A1B-4D07BCAF2535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3A34D822-9F98-46FD-9C56-89E978C0B272}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D1395CAA-C2E5-497D-87AD-FD08627C7CC7}"/>
   </bookViews>
@@ -104,9 +104,6 @@
     <t>12. Gym</t>
   </si>
   <si>
-    <t>13. Outside</t>
-  </si>
-  <si>
     <t>14. Public parking</t>
   </si>
   <si>
@@ -116,42 +113,15 @@
     <t>"2,3,4,5,6"</t>
   </si>
   <si>
-    <t>"1,7"</t>
-  </si>
-  <si>
     <t>"1,13"</t>
   </si>
   <si>
     <t>"1"</t>
   </si>
   <si>
-    <t>"1,9"</t>
-  </si>
-  <si>
     <t>"2,3"</t>
   </si>
   <si>
-    <t>"11,13,14"</t>
-  </si>
-  <si>
-    <t>"6,13,14"</t>
-  </si>
-  <si>
-    <t>"13"</t>
-  </si>
-  <si>
-    <t>"8,13"</t>
-  </si>
-  <si>
-    <t>"13,14"</t>
-  </si>
-  <si>
-    <t>"4,8,9,10,11,12"</t>
-  </si>
-  <si>
-    <t>"8,9,12"</t>
-  </si>
-  <si>
     <t>Housing_entree</t>
   </si>
   <si>
@@ -191,7 +161,37 @@
     <t>Gym</t>
   </si>
   <si>
-    <t>Outside</t>
+    <t>"11,14"</t>
+  </si>
+  <si>
+    <t>"8"</t>
+  </si>
+  <si>
+    <t>"6,14"</t>
+  </si>
+  <si>
+    <t>"14"</t>
+  </si>
+  <si>
+    <t>13. Atrium</t>
+  </si>
+  <si>
+    <t>"1,7,13"</t>
+  </si>
+  <si>
+    <t>"1,9,13"</t>
+  </si>
+  <si>
+    <t>"2,3,5,6"</t>
+  </si>
+  <si>
+    <t>"8,9,10,12"</t>
+  </si>
+  <si>
+    <t>Atrium</t>
+  </si>
+  <si>
+    <t>Area</t>
   </si>
 </sst>
 </file>
@@ -207,18 +207,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -238,7 +232,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -556,7 +550,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K21" sqref="K21"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,13 +613,13 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="I2">
         <v>450</v>
@@ -634,7 +628,7 @@
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -654,13 +648,13 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="I3">
         <v>12500</v>
@@ -669,7 +663,7 @@
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -689,13 +683,13 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="G4">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="I4">
         <v>10000</v>
@@ -704,7 +698,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -724,13 +718,13 @@
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="I5">
         <v>16000</v>
@@ -739,7 +733,7 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -759,13 +753,13 @@
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="I6">
         <v>6500</v>
@@ -774,7 +768,7 @@
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -794,13 +788,13 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="I7">
         <v>6500</v>
@@ -809,7 +803,7 @@
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -829,13 +823,13 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="G8">
         <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="I8">
         <v>2000</v>
@@ -844,7 +838,7 @@
         <v>0.7</v>
       </c>
       <c r="K8" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -864,13 +858,13 @@
         <v>8</v>
       </c>
       <c r="F9" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="G9">
         <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="I9">
         <v>800</v>
@@ -879,7 +873,7 @@
         <v>0.9</v>
       </c>
       <c r="K9" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -899,13 +893,13 @@
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="G10">
         <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="I10">
         <v>1000</v>
@@ -914,7 +908,7 @@
         <v>0.8</v>
       </c>
       <c r="K10" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -934,13 +928,13 @@
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="G11">
         <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="I11">
         <v>200</v>
@@ -949,7 +943,7 @@
         <v>0.7</v>
       </c>
       <c r="K11" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -969,13 +963,13 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="G12">
         <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="I12">
         <v>200</v>
@@ -984,7 +978,7 @@
         <v>0.9</v>
       </c>
       <c r="K12" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1004,13 +998,13 @@
         <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="G13">
         <v>3</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="I13">
         <v>950</v>
@@ -1019,12 +1013,12 @@
         <v>0.8</v>
       </c>
       <c r="K13" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
@@ -1039,21 +1033,27 @@
         <v>13</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G14" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="G14" s="2">
+        <v>1</v>
+      </c>
       <c r="H14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+        <v>50</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2000</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.9</v>
+      </c>
       <c r="K14" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1068,13 +1068,13 @@
         <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="I15">
         <v>2000</v>
@@ -1083,96 +1083,96 @@
         <v>0.9</v>
       </c>
       <c r="K15" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="I17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" t="str">
-        <f>CONCATENATE(B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2)</f>
+        <f t="shared" ref="B20:B33" si="0">CONCATENATE(B2,",",C2,",",D2,",",E2,",",F2,",",G2,",",H2,",",I2,",",J2,",",K2)</f>
         <v>0,0,0,1,"2,3,4,5,6",1,Housing_entree,450,1,Housing_entree</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" t="str">
-        <f>CONCATENATE(B3,",",C3,",",D3,",",E3,",",F3,",",G3,",",H3,",",I3,",",J3,",",K3)</f>
-        <v>0,0,0,2,"1,7",1,Starter_houses,12500,1,Starter_houses</v>
+        <f t="shared" si="0"/>
+        <v>0,0,0,2,"1,7,13",1,Starter_houses,12500,1,Starter_houses</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" t="str">
-        <f>CONCATENATE(B4,",",C4,",",D4,",",E4,",",F4,",",G4,",",H4,",",I4,",",J4,",",K4)</f>
-        <v>0,0,0,3,"1,7",1,Student_houses,10000,1,Student_houses</v>
+        <f t="shared" si="0"/>
+        <v>0,0,0,3,"1,7,13",1,Student_houses,10000,1,Student_houses</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" t="str">
-        <f>CONCATENATE(B5,",",C5,",",D5,",",E5,",",F5,",",G5,",",H5,",",I5,",",J5,",",K5)</f>
-        <v>0,0,0,4,"1,13",1,Private_parking,16000,1,Private_parking</v>
+        <f t="shared" si="0"/>
+        <v>0,0,0,4,"1",1,Private_parking,16000,1,Private_parking</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" t="str">
-        <f>CONCATENATE(B6,",",C6,",",D6,",",E6,",",F6,",",G6,",",H6,",",I6,",",J6,",",K6)</f>
-        <v>0,0,0,5,"1",1,Independent_elderly_houses,6500,1,Independent_elderly_houses</v>
+        <f t="shared" si="0"/>
+        <v>0,0,0,5,"1,13",1,Independent_elderly_houses,6500,1,Independent_elderly_houses</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" t="str">
-        <f>CONCATENATE(B7,",",C7,",",D7,",",E7,",",F7,",",G7,",",H7,",",I7,",",J7,",",K7)</f>
-        <v>0,0,0,6,"1,9",1,Dependent_elderly_houses,6500,1,Dependent_elderly_houses</v>
+        <f t="shared" si="0"/>
+        <v>0,0,0,6,"1,9,13",1,Dependent_elderly_houses,6500,1,Dependent_elderly_houses</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" t="str">
-        <f>CONCATENATE(B8,",",C8,",",D8,",",E8,",",F8,",",G8,",",H8,",",I8,",",J8,",",K8)</f>
+        <f t="shared" si="0"/>
         <v>0,0,0,7,"2,3",1,Shared_workspaces,2000,0,7,Shared_workspaces</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" t="str">
-        <f>CONCATENATE(B9,",",C9,",",D9,",",E9,",",F9,",",G9,",",H9,",",I9,",",J9,",",K9)</f>
-        <v>0,0,0,8,"11,13,14",2,Supermarket,800,0,9,Supermarket</v>
+        <f t="shared" si="0"/>
+        <v>0,0,0,8,"11,14",2,Supermarket,800,0,9,Supermarket</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" t="str">
-        <f>CONCATENATE(B10,",",C10,",",D10,",",E10,",",F10,",",G10,",",H10,",",I10,",",J10,",",K10)</f>
-        <v>0,0,0,9,"6,13,14",3,Care_center_elderly,1000,0,8,Care_center_elderly</v>
+        <f t="shared" si="0"/>
+        <v>0,0,0,9,"6,14",3,Care_center_elderly,1000,0,8,Care_center_elderly</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" t="str">
-        <f>CONCATENATE(B11,",",C11,",",D11,",",E11,",",F11,",",G11,",",H11,",",I11,",",J11,",",K11)</f>
-        <v>0,0,0,10,"13",3,Cafe,200,0,7,Cafe</v>
+        <f t="shared" si="0"/>
+        <v>0,0,0,10,"14",3,Cafe,200,0,7,Cafe</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" t="str">
-        <f>CONCATENATE(B12,",",C12,",",D12,",",E12,",",F12,",",G12,",",H12,",",I12,",",J12,",",K12)</f>
-        <v>0,0,0,11,"8,13",2,Loading_dock,200,0,9,Loading_dock</v>
+        <f t="shared" si="0"/>
+        <v>0,0,0,11,"8",2,Loading_dock,200,0,9,Loading_dock</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" t="str">
-        <f>CONCATENATE(B13,",",C13,",",D13,",",E13,",",F13,",",G13,",",H13,",",I13,",",J13,",",K13)</f>
-        <v>0,0,0,12,"13,14",3,Gym,950,0,8,Gym</v>
+        <f t="shared" si="0"/>
+        <v>0,0,0,12,"14",3,Gym,950,0,8,Gym</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" t="str">
-        <f>CONCATENATE(B14,",",C14,",",D14,",",E14,",",F14,",",G14,",",H14,",",I14,",",J14,",",K14)</f>
-        <v>0,0,0,13,"4,8,9,10,11,12",,Outside,,,Outside</v>
+        <f t="shared" si="0"/>
+        <v>0,0,0,13,"2,3,5,6",1,Atrium,2000,0,9,Area</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="str">
-        <f>CONCATENATE(B15,",",C15,",",D15,",",E15,",",F15,",",G15,",",H15,",",I15,",",J15,",",K15)</f>
-        <v>0,0,0,14,"8,9,12",2,Public_parking,2000,0,9,Public_parking</v>
+        <f t="shared" si="0"/>
+        <v>0,0,0,14,"8,9,10,12",2,Public_parking,2000,0,9,Public_parking</v>
       </c>
     </row>
   </sheetData>

</xml_diff>